<commit_message>
Actualizacion de caracteristicas de usuario y entidad en el frontend y ajuste del controlador excel para los nuevos parametros de la plantilla
</commit_message>
<xml_diff>
--- a/src/excel/U_PLANTILLA_CERTIFICADO_QR1.xlsx
+++ b/src/excel/U_PLANTILLA_CERTIFICADO_QR1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\_OTIC\_SISTEMAS\SISTEMA-QR\qr-code-api\src\excel\masivo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\_OTIC\_SISTEMAS\SISTEMA-QR\qr-code-api\src\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF58382-414B-42A7-B727-2857FCEB11DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D6BF7C-8424-4220-B342-2DD02938A6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="13740" windowHeight="23640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MASIVO" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>NOMBRES</t>
   </si>
@@ -109,111 +109,9 @@
     <t>CORREO_PERSONAL</t>
   </si>
   <si>
-    <t>ILASACA</t>
-  </si>
-  <si>
-    <t>CORONADO</t>
-  </si>
-  <si>
-    <t>NÚÑEZ</t>
-  </si>
-  <si>
-    <t>LANDEO</t>
-  </si>
-  <si>
-    <t>BUSTAMANTE</t>
-  </si>
-  <si>
-    <t>CALISAYA</t>
-  </si>
-  <si>
-    <t>CASA</t>
-  </si>
-  <si>
-    <t>MIÑANO</t>
-  </si>
-  <si>
-    <t>SANCHEZ</t>
-  </si>
-  <si>
-    <t>CASTRO</t>
-  </si>
-  <si>
-    <t>ZUASNABAR</t>
-  </si>
-  <si>
-    <t>FARIS</t>
-  </si>
-  <si>
-    <t>POMA</t>
-  </si>
-  <si>
-    <t>HUAMAN</t>
-  </si>
-  <si>
-    <t>AGUILAR</t>
-  </si>
-  <si>
-    <t>LÓPEZ</t>
-  </si>
-  <si>
-    <t>CUCHO</t>
-  </si>
-  <si>
-    <t>VEGA</t>
-  </si>
-  <si>
-    <t>FUENTES</t>
-  </si>
-  <si>
-    <t>MARLON MARK</t>
-  </si>
-  <si>
-    <t>PATRICIA JANETH</t>
-  </si>
-  <si>
-    <t>MÁXIMO MANUEL</t>
-  </si>
-  <si>
-    <t>ERICK ELOY</t>
-  </si>
-  <si>
-    <t>YONATAN ANIBAL</t>
-  </si>
-  <si>
-    <t>HECTOR RAUL</t>
-  </si>
-  <si>
-    <t>JULIO CÉSAR</t>
-  </si>
-  <si>
-    <t>NELSON RUDY</t>
-  </si>
-  <si>
-    <t>WHENER ALBERTO</t>
-  </si>
-  <si>
-    <t>JULIO CESAR</t>
-  </si>
-  <si>
-    <t>PROGRAMA DE ESTUDIOS GENERALES</t>
-  </si>
-  <si>
     <t>PONENTE</t>
   </si>
   <si>
-    <t>DOCENTE</t>
-  </si>
-  <si>
-    <t>abc@untels.edu.pe</t>
-  </si>
-  <si>
-    <t>xyz@gmail.com</t>
-  </si>
-  <si>
-    <t>EVENTO_ID</t>
-  </si>
-  <si>
     <t>FECHA_EMISION</t>
   </si>
   <si>
@@ -224,13 +122,16 @@
   </si>
   <si>
     <t>DIA - MES - AÑO</t>
+  </si>
+  <si>
+    <t>HORAS_ASISTENCIA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +165,29 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -560,7 +484,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -622,9 +546,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -641,19 +565,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -936,621 +866,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="21" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
+      <c r="L1" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="35">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="32" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="34"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="35">
         <v>2</v>
       </c>
-      <c r="F2" s="32">
-        <v>44009270</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2" s="32">
-        <v>1</v>
-      </c>
-      <c r="M2" s="34">
-        <v>45651</v>
-      </c>
-      <c r="N2" s="29"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
-        <v>2</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="32">
-        <v>42949905</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="L3" s="32">
-        <v>1</v>
-      </c>
-      <c r="M3" s="34">
-        <v>45651</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="34"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="35">
         <v>3</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="32">
-        <v>71401195</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="K4" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="L4" s="32">
-        <v>1</v>
-      </c>
-      <c r="M4" s="34">
-        <v>45651</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="34"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="35">
         <v>4</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="32">
-        <v>70439188</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="L5" s="32">
-        <v>1</v>
-      </c>
-      <c r="M5" s="34">
-        <v>45651</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="34"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="35">
         <v>5</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="32">
-        <v>42972319</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="K6" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="L6" s="32">
-        <v>1</v>
-      </c>
-      <c r="M6" s="34">
-        <v>45651</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="34"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="35">
         <v>6</v>
       </c>
-      <c r="B7" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="32">
-        <v>44484577</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J7" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="K7" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" s="32">
-        <v>1</v>
-      </c>
-      <c r="M7" s="34">
-        <v>45651</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="34"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="35">
         <v>7</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="32">
-        <v>43225336</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J8" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="K8" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="L8" s="32">
-        <v>1</v>
-      </c>
-      <c r="M8" s="34">
-        <v>45651</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="34"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="35">
         <v>8</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="32">
-        <v>42002308</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="K9" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="L9" s="32">
-        <v>1</v>
-      </c>
-      <c r="M9" s="34">
-        <v>45651</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="34"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="35">
         <v>9</v>
       </c>
-      <c r="B10" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="32">
-        <v>42205309</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="K10" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="L10" s="32">
-        <v>1</v>
-      </c>
-      <c r="M10" s="34">
-        <v>45651</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="34"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="35">
         <v>10</v>
       </c>
-      <c r="B11" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="32">
-        <v>10218557</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J11" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="K11" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="L11" s="32">
-        <v>1</v>
-      </c>
-      <c r="M11" s="34">
-        <v>45651</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="34"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="36"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="29"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="36"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="29"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="36"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="29"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="36"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="29"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="36"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="29"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="29"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="29"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="29"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="29"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="36"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="29"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="36"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{2FB69C71-E92C-4F0C-83C9-FE00DE2B365C}"/>
-    <hyperlink ref="J3:J11" r:id="rId2" display="abc@untels.edu.pe" xr:uid="{0AA8F9EB-6D51-4480-9530-B67186DC0BF8}"/>
-    <hyperlink ref="K2" r:id="rId3" xr:uid="{1EB8D1AD-D937-491D-92CD-2B8CA4CA2DD2}"/>
-    <hyperlink ref="K3:K11" r:id="rId4" display="xyz@gmail.com" xr:uid="{70B6052E-DCA8-4516-B01F-EAB252A40A51}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1558,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6612173-2DB8-465F-8A72-D7E717669F7E}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,7 +1364,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="C8" s="17">
         <v>1</v>
@@ -1656,7 +1373,7 @@
     <row r="9" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="6" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="C9" s="9">
         <v>2</v>
@@ -1665,7 +1382,7 @@
     <row r="10" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25"/>
       <c r="B10" s="7" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="C10" s="10">
         <v>3</v>
@@ -1729,13 +1446,13 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>